<commit_message>
hoan thanh mot so chuc nang
</commit_message>
<xml_diff>
--- a/file/datamhthuocnganh.xlsx
+++ b/file/datamhthuocnganh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualStudioCode\data_baitaplon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF05B9D9-54C0-444C-9800-3367417C0526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0293FB99-5F4A-4403-B339-B4CB90980495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -375,7 +375,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>